<commit_message>
Grub: GN Sitzung am 27.05.2014
</commit_message>
<xml_diff>
--- a/2014/GN-Checkliste 2014.xlsx
+++ b/2014/GN-Checkliste 2014.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="116">
   <si>
     <t>Musik</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>aw       Michael</t>
+  </si>
+  <si>
+    <t>Geschirrmobil</t>
+  </si>
+  <si>
+    <t>am DO herstellen</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -506,7 +512,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -818,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O47" sqref="O47"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +922,7 @@
       <c r="I4" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1" t="s">
         <v>82</v>
       </c>
@@ -943,7 +948,7 @@
       <c r="I5" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="20"/>
       <c r="K5" s="1" t="s">
         <v>83</v>
       </c>
@@ -993,7 +998,7 @@
       <c r="I7" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J7" s="21"/>
+      <c r="J7" s="20"/>
       <c r="K7" s="1" t="s">
         <v>46</v>
       </c>
@@ -1057,7 +1062,7 @@
     </row>
     <row r="10" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="21"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1067,7 +1072,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="19"/>
+      <c r="J10" s="18"/>
       <c r="K10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1119,7 +1124,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="20"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1147,7 +1152,7 @@
       <c r="I13" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="23"/>
       <c r="K13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1189,7 +1194,7 @@
       <c r="A15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1218,7 +1223,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="21"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1257,7 +1262,7 @@
       <c r="G17" s="14"/>
       <c r="H17" s="1"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="21"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1288,7 +1293,7 @@
         <v>48</v>
       </c>
       <c r="J18" s="1"/>
-      <c r="K18" s="21"/>
+      <c r="K18" s="20"/>
       <c r="L18" s="1" t="s">
         <v>31</v>
       </c>
@@ -1325,7 +1330,7 @@
     </row>
     <row r="20" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
-      <c r="B20" s="21"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="1" t="s">
         <v>71</v>
       </c>
@@ -1340,7 +1345,7 @@
         <v>48</v>
       </c>
       <c r="J20" s="1"/>
-      <c r="K20" s="15"/>
+      <c r="K20" s="20"/>
       <c r="L20" s="1" t="s">
         <v>33</v>
       </c>
@@ -1381,7 +1386,7 @@
       <c r="A22" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="21"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1393,7 +1398,7 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="21"/>
+      <c r="J22" s="20"/>
       <c r="K22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1407,7 +1412,7 @@
     </row>
     <row r="23" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="B23" s="21"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="1" t="s">
         <v>53</v>
       </c>
@@ -1417,7 +1422,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="23"/>
+      <c r="J23" s="22"/>
       <c r="K23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1433,7 +1438,7 @@
     </row>
     <row r="24" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
-      <c r="B24" s="21"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1447,7 +1452,7 @@
       <c r="I24" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="J24" s="15"/>
+      <c r="J24" s="20"/>
       <c r="K24" s="1" t="s">
         <v>64</v>
       </c>
@@ -1475,7 +1480,7 @@
       <c r="I25" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="J25" s="15"/>
+      <c r="J25" s="20"/>
       <c r="K25" s="1" t="s">
         <v>97</v>
       </c>
@@ -1503,7 +1508,7 @@
       <c r="I26" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="15"/>
+      <c r="J26" s="20"/>
       <c r="K26" s="1" t="s">
         <v>102</v>
       </c>
@@ -1517,7 +1522,7 @@
     </row>
     <row r="27" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
-      <c r="B27" s="17"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="1" t="s">
         <v>60</v>
       </c>
@@ -1531,7 +1536,7 @@
       <c r="I27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="J27" s="21"/>
+      <c r="J27" s="20"/>
       <c r="K27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1545,44 +1550,36 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="25"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="14" t="s">
         <v>92</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="29" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="18"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="14" t="s">
         <v>106</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J29" s="22"/>
-      <c r="K29" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="14" t="s">
-        <v>94</v>
-      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
     <row r="30" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1599,23 +1596,23 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J30" s="15"/>
+        <v>59</v>
+      </c>
+      <c r="J30" s="21"/>
       <c r="K30" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
       <c r="O30" s="14" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="P30" s="1"/>
     </row>
     <row r="31" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
-      <c r="B31" s="21"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="1" t="s">
         <v>12</v>
       </c>
@@ -1625,17 +1622,17 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J31" s="15"/>
+        <v>61</v>
+      </c>
+      <c r="J31" s="20"/>
       <c r="K31" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="1" t="s">
-        <v>66</v>
+      <c r="O31" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="P31" s="1"/>
     </row>
@@ -1643,7 +1640,7 @@
       <c r="A32" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="21"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1655,17 +1652,17 @@
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J32" s="21"/>
+        <v>59</v>
+      </c>
+      <c r="J32" s="20"/>
       <c r="K32" s="1" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-      <c r="O32" s="14" t="s">
-        <v>79</v>
+      <c r="O32" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="P32" s="1"/>
     </row>
@@ -1682,15 +1679,19 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="1"/>
+      <c r="I33" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J33" s="20"/>
+      <c r="K33" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
+      <c r="O33" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="P33" s="1"/>
     </row>
     <row r="34" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1706,13 +1707,11 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J34" s="15"/>
-      <c r="K34" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="I34" s="8"/>
+      <c r="J34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -1737,7 +1736,7 @@
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -1758,9 +1757,13 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
+      <c r="I36" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J36" s="15"/>
+      <c r="K36" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -1805,7 +1808,17 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+    </row>
     <row r="40" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>